<commit_message>
Added code smells for Jfree Chart
</commit_message>
<xml_diff>
--- a/Projects/Jfree Chart/Metric 6/Version 1.0.15/Feature Envy.xlsx
+++ b/Projects/Jfree Chart/Metric 6/Version 1.0.15/Feature Envy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karansharma/Desktop/Jfree/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karansharma/Desktop/SOEN6611_Project_Group_C/Projects/Jfree Chart/Metric 6/Version 1.0.15/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{560A1D46-6A6F-5944-A612-27DBECB86393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3E60BA-221E-6342-815E-CAA520359C3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15520" xr2:uid="{73D90F54-8A39-584F-9C33-DE334C1B6BB5}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Feature_envy" localSheetId="0">Sheet1!$A$1:$E$30</definedName>
+    <definedName name="fe_15" localSheetId="0">Sheet1!$A$2:$E$31</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,8 +37,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{B2B5F975-7004-C04F-8001-CAE190F0E41A}" name="Feature envy" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/karansharma/Desktop/Jfree/Feature envy.txt">
+  <connection id="1" xr16:uid="{911A338B-BF93-E84F-BE16-65AF5D7B58DA}" name="fe 15" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/karansharma/Desktop/type/fe 15.txt">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>Refactoring Type</t>
   </si>
@@ -196,6 +196,24 @@
   </si>
   <si>
     <t>org.jfree.chart.plot.SpiderWebPlot</t>
+  </si>
+  <si>
+    <t>Source/Target accessed members</t>
+  </si>
+  <si>
+    <t>Rate it!</t>
+  </si>
+  <si>
+    <t>0/4</t>
+  </si>
+  <si>
+    <t>0/3</t>
+  </si>
+  <si>
+    <t>0/2</t>
+  </si>
+  <si>
+    <t>0/1</t>
   </si>
 </sst>
 </file>
@@ -261,7 +279,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Feature envy" connectionId="1" xr16:uid="{DED3F144-5440-ED42-89C3-A6DB18D9AA95}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fe 15" connectionId="1" xr16:uid="{FEE6A23E-B9C3-7444-83DB-381B3FE6FA54}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89CE7795-56C9-8749-8178-A1B6B072806C}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,117 +594,141 @@
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -694,21 +736,27 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -716,32 +764,41 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -749,7 +806,10 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -757,10 +817,13 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,10 +831,13 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -779,144 +845,182 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="D20" s="1">
+        <v>43952</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1">
+        <v>43891</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D22" s="1">
+        <v>43891</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43891</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1">
+        <v>43891</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D25" s="1">
+        <v>43891</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1">
+        <v>43891</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D27" s="1">
+        <v>43891</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="D28" s="1">
+        <v>43862</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="D29" s="1">
+        <v>43862</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3</v>
       </c>
       <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="1">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
         <v>46</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D31" s="1">
+        <v>43892</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>